<commit_message>
Update Dataset 2: Include all OECD countries and add national legal sources
</commit_message>
<xml_diff>
--- a/output/analysis_1.xlsx
+++ b/output/analysis_1.xlsx
@@ -639,7 +639,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:F7"/>
+  <dimension ref="A1:F8"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -807,6 +807,28 @@
       </c>
       <c r="F7">
         <v>0.7</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>EU_OECD</t>
+        </is>
+      </c>
+      <c r="B8">
+        <v>516</v>
+      </c>
+      <c r="C8">
+        <v>388</v>
+      </c>
+      <c r="D8">
+        <v>516</v>
+      </c>
+      <c r="E8">
+        <v>0.751937984496124</v>
+      </c>
+      <c r="F8">
+        <v>1</v>
       </c>
     </row>
   </sheetData>

</xml_diff>